<commit_message>
format power data, more analysis
</commit_message>
<xml_diff>
--- a/force_calculations.xlsx
+++ b/force_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C389F41-EEB5-4ABB-A745-7DAB84E33421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF03FAA-3420-40AC-B211-40AE2794E7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
   </bookViews>
@@ -4655,7 +4655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D247D-C69E-4F80-AEFB-C1F8182EA819}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pcb finalized, very exciting
</commit_message>
<xml_diff>
--- a/force_calculations.xlsx
+++ b/force_calculations.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF03FAA-3420-40AC-B211-40AE2794E7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E9C9DD-9151-4909-B1D9-6504AD0B746F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Safety Calculations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -151,9 +151,6 @@
     <t>Part No.</t>
   </si>
   <si>
-    <t>Pulling Force (kg)</t>
-  </si>
-  <si>
     <t>Normal Force (N)</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>D83-N52</t>
+  </si>
+  <si>
+    <t>Holding Strength (kg)</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
           </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$11</c:f>
+              <c:f>'Safety Calculations'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -969,7 +969,7 @@
           </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$12:$F$21</c:f>
+              <c:f>'Safety Calculations'!$F$12:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1358,7 +1358,7 @@
           </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$22:$F$31</c:f>
+              <c:f>'Safety Calculations'!$F$22:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1747,7 +1747,7 @@
           </c:trendline>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$32:$F$41</c:f>
+              <c:f>'Safety Calculations'!$F$32:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4656,14 +4656,15 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4676,16 +4677,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4714,7 +4715,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5">
         <v>85</v>
@@ -4754,7 +4755,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5">
         <v>65</v>
@@ -4794,7 +4795,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="17">
         <v>45</v>
@@ -4889,7 +4890,7 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
         <v>90</v>
@@ -4913,7 +4914,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>85</v>
@@ -4953,7 +4954,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="5">
         <v>65</v>
@@ -4993,7 +4994,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="17">
         <v>45</v>
@@ -5088,7 +5089,7 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
         <v>90</v>
@@ -5112,7 +5113,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1">
         <v>85</v>
@@ -5152,7 +5153,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="5">
         <v>65</v>
@@ -5192,7 +5193,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="17">
         <v>45</v>
@@ -5287,7 +5288,7 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1">
         <v>90</v>
@@ -5311,7 +5312,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1">
         <v>85</v>
@@ -5351,7 +5352,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" s="5">
         <v>65</v>
@@ -5391,7 +5392,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="17">
         <v>45</v>

</xml_diff>

<commit_message>
multi magnet versions exported to printable files
four magnet sizes have been chosen for testing purposes. Their models
and corresponding mounts have been categorized for printing and testing.
</commit_message>
<xml_diff>
--- a/force_calculations.xlsx
+++ b/force_calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA967689-0795-4A52-976A-C75ED4829B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA72389A-B214-49D5-AFF2-73F21F05A338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Safety Calculations" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -404,7 +404,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3237,7 +3236,7 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="6667499" y="1194954"/>
+    <xdr:pos x="6684818" y="1376795"/>
     <xdr:ext cx="4828430" cy="3442673"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3597,10 +3596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D247D-C69E-4F80-AEFB-C1F8182EA819}">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3612,7 @@
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>8.2816597543881427E-16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -3677,7 +3676,7 @@
         <v>1.1782967267112507</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>9.25</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>3.4990882303395447</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>5.7135617087130504</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>1.35</v>
       </c>
@@ -3736,12 +3735,8 @@
         <f t="shared" si="1"/>
         <v>7.7544315057690394</v>
       </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>9</v>
       </c>
@@ -3753,7 +3748,7 @@
         <v>2.9730626027161655</v>
       </c>
       <c r="D7" s="18">
-        <f t="shared" si="0"/>
+        <f>C7*9.8</f>
         <v>29.136013506618426</v>
       </c>
       <c r="E7" s="19"/>
@@ -3761,12 +3756,8 @@
         <f t="shared" si="1"/>
         <v>9.5596868254539089</v>
       </c>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
     </row>
-    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <f>A6*4</f>
         <v>5.4</v>
@@ -3786,12 +3777,8 @@
         <f t="shared" si="1"/>
         <v>11.074475898382305</v>
       </c>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>25</v>
       </c>
@@ -3807,12 +3794,8 @@
         <f t="shared" si="1"/>
         <v>12.252772625093558</v>
       </c>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="22"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>15</v>
       </c>
@@ -3828,12 +3811,8 @@
         <f t="shared" si="1"/>
         <v>13.058775055793454</v>
       </c>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
     </row>
-    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="9">
         <v>0</v>
@@ -3851,12 +3830,8 @@
         <f t="shared" si="1"/>
         <v>13.519438760596316</v>
       </c>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
-      <c r="T11" s="22"/>
     </row>
-    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -3879,12 +3854,8 @@
         <f t="shared" si="1"/>
         <v>1.7181086560725241E-15</v>
       </c>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
@@ -3903,12 +3874,8 @@
         <f t="shared" si="1"/>
         <v>2.4444880200636652</v>
       </c>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-      <c r="T13" s="22"/>
     </row>
-    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>19.190000000000001</v>
       </c>
@@ -3927,12 +3894,8 @@
         <f t="shared" si="1"/>
         <v>7.2591895286719872</v>
       </c>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
@@ -3952,7 +3915,7 @@
         <v>11.853324236778752</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>3.49</v>
       </c>

</xml_diff>

<commit_message>
re-arrange files and folders, update components
</commit_message>
<xml_diff>
--- a/force_calculations.xlsx
+++ b/force_calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA72389A-B214-49D5-AFF2-73F21F05A338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365B7E7A-5A09-444F-BB27-637D571F5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Safety Calculations" sheetId="1" r:id="rId1"/>
@@ -3236,8 +3236,8 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="6684818" y="1376795"/>
-    <xdr:ext cx="4828430" cy="3442673"/>
+    <xdr:pos x="6283037" y="327313"/>
+    <xdr:ext cx="6166138" cy="4216112"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5">
@@ -3598,8 +3598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D247D-C69E-4F80-AEFB-C1F8182EA819}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update testing and force calculations
</commit_message>
<xml_diff>
--- a/force_calculations.xlsx
+++ b/force_calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MaxYoung\OneDrive - Tiger Optics\Documents\commapogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365B7E7A-5A09-444F-BB27-637D571F5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474A5CD8-9C75-48C8-AB9F-D99D0352E514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Safety Calculations" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{E0D2AB1C-C41C-4098-BBE1-3588EDA2393F}">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{E0D2AB1C-C41C-4098-BBE1-3588EDA2393F}">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{ADC1AD87-6389-4E6D-98C7-14C255B92D4A}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{ADC1AD87-6389-4E6D-98C7-14C255B92D4A}">
       <text>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{637BC005-84ED-4B36-AD16-D2D1D76DC17F}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{637BC005-84ED-4B36-AD16-D2D1D76DC17F}">
       <text>
         <r>
           <rPr>
@@ -371,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -404,6 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -565,10 +566,10 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$2:$B$11</c:f>
+              <c:f>'Safety Calculations'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
@@ -591,12 +592,15 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -604,10 +608,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$2:$F$11</c:f>
+              <c:f>'Safety Calculations'!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>8.2816597543881427E-16</c:v>
                 </c:pt>
@@ -630,12 +634,15 @@
                   <c:v>11.074475898382305</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>11.991888639138484</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>12.252772625093558</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>13.058775055793454</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>13.519438760596316</c:v>
                 </c:pt>
               </c:numCache>
@@ -653,7 +660,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Safety Calculations'!$A$12</c:f>
+              <c:f>'Safety Calculations'!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -712,10 +719,10 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$12:$B$21</c:f>
+              <c:f>'Safety Calculations'!$B$13:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
@@ -738,12 +745,15 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -751,10 +761,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$12:$F$21</c:f>
+              <c:f>'Safety Calculations'!$F$13:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.7181086560725241E-15</c:v>
                 </c:pt>
@@ -777,12 +787,15 @@
                   <c:v>22.975047836752047</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>24.878307349737028</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>25.419535856815717</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>27.091664142775826</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>28.047354574685766</c:v>
                 </c:pt>
               </c:numCache>
@@ -800,7 +813,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Safety Calculations'!$A$22</c:f>
+              <c:f>'Safety Calculations'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -857,7 +870,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$22:$B$31</c:f>
+              <c:f>'Safety Calculations'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -896,7 +909,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$22:$F$31</c:f>
+              <c:f>'Safety Calculations'!$F$24:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -945,7 +958,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Safety Calculations'!$A$32</c:f>
+              <c:f>'Safety Calculations'!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1004,7 +1017,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$32:$B$41</c:f>
+              <c:f>'Safety Calculations'!$B$34:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1043,7 +1056,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$32:$F$41</c:f>
+              <c:f>'Safety Calculations'!$F$34:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1435,10 +1448,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$2:$B$11</c:f>
+              <c:f>'Safety Calculations'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
@@ -1461,12 +1474,15 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1474,10 +1490,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$2:$F$11</c:f>
+              <c:f>'Safety Calculations'!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>8.2816597543881427E-16</c:v>
                 </c:pt>
@@ -1500,12 +1516,15 @@
                   <c:v>11.074475898382305</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>11.991888639138484</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>12.252772625093558</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>13.058775055793454</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>13.519438760596316</c:v>
                 </c:pt>
               </c:numCache>
@@ -1523,7 +1542,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Safety Calculations'!$A$12</c:f>
+              <c:f>'Safety Calculations'!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1558,10 +1577,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$12:$B$21</c:f>
+              <c:f>'Safety Calculations'!$B$13:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
@@ -1584,12 +1603,15 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1597,10 +1619,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$12:$F$21</c:f>
+              <c:f>'Safety Calculations'!$F$13:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.7181086560725241E-15</c:v>
                 </c:pt>
@@ -1623,12 +1645,15 @@
                   <c:v>22.975047836752047</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>24.878307349737028</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>25.419535856815717</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>27.091664142775826</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>28.047354574685766</c:v>
                 </c:pt>
               </c:numCache>
@@ -1646,7 +1671,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Safety Calculations'!$A$22</c:f>
+              <c:f>'Safety Calculations'!$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1681,7 +1706,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$22:$B$31</c:f>
+              <c:f>'Safety Calculations'!$B$24:$B$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1720,7 +1745,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$22:$F$31</c:f>
+              <c:f>'Safety Calculations'!$F$24:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1769,7 +1794,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Safety Calculations'!$A$32</c:f>
+              <c:f>'Safety Calculations'!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1804,7 +1829,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$B$32:$B$41</c:f>
+              <c:f>'Safety Calculations'!$B$34:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1843,7 +1868,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Safety Calculations'!$F$32:$F$41</c:f>
+              <c:f>'Safety Calculations'!$F$34:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3236,7 +3261,7 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="6283037" y="327313"/>
+    <xdr:pos x="6635462" y="1565563"/>
     <xdr:ext cx="6166138" cy="4216112"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3596,10 +3621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D247D-C69E-4F80-AEFB-C1F8182EA819}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3644,7 +3669,7 @@
         <v>2.5755961836147122E-16</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:D14" si="0">C2*9.8</f>
+        <f t="shared" ref="D2:D15" si="0">C2*9.8</f>
         <v>2.5240842599424181E-15</v>
       </c>
       <c r="E2" s="2">
@@ -3652,7 +3677,7 @@
         <v>3.0478000000000001</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F14" si="1">D2/$E$2</f>
+        <f t="shared" ref="F2:F15" si="1">D2/$E$2</f>
         <v>8.2816597543881427E-16</v>
       </c>
     </row>
@@ -3664,7 +3689,7 @@
         <v>85</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C11" si="2">($A$4/2.2)*COS(RADIANS(B3))</f>
+        <f t="shared" ref="C3:C12" si="2">($A$4/2.2)*COS(RADIANS(B3))</f>
         <v>0.36645028200719898</v>
       </c>
       <c r="D3" s="2">
@@ -3779,651 +3804,687 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="1">
-        <v>25</v>
+      <c r="A9" s="22"/>
+      <c r="B9" s="5">
+        <v>27.5</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="2"/>
-        <v>3.8106122864040959</v>
+        <f>($A$4/2.2)*COS(RADIANS(B9))</f>
+        <v>3.7294773667720684</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>37.344000406760145</v>
+        <v>36.548878194366274</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="1"/>
-        <v>12.252772625093558</v>
+        <v>11.991888639138484</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="2"/>
-        <v>4.0612790423517637</v>
+        <v>3.8106122864040959</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>39.80053461504729</v>
+        <v>37.344000406760145</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="1"/>
+        <v>12.252772625093558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="2"/>
+        <v>4.0612790423517637</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>39.80053461504729</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
         <v>13.058775055793454</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
         <v>0</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C12" s="10">
         <f t="shared" si="2"/>
         <v>4.2045454545454541</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D12" s="10">
         <f t="shared" si="0"/>
         <v>41.204545454545453</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="11">
+      <c r="E12" s="8"/>
+      <c r="F12" s="11">
         <f t="shared" si="1"/>
         <v>13.519438760596316</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>90</v>
       </c>
-      <c r="C12" s="2">
-        <f>($A$14/2.2)*COS(RADIANS(B12))</f>
+      <c r="C13" s="2">
+        <f>($A$15/2.2)*COS(RADIANS(B13))</f>
         <v>5.3433179203855495E-16</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>5.236451561977839E-15</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E13" s="2">
         <f>0.311*9.8</f>
         <v>3.0478000000000001</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
         <v>1.7181086560725241E-15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B14" s="1">
         <v>85</v>
       </c>
-      <c r="C13" s="2">
-        <f t="shared" ref="C13:C21" si="3">($A$14/2.2)*COS(RADIANS(B13))</f>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:C23" si="3">($A$15/2.2)*COS(RADIANS(B14))</f>
         <v>0.76023577423979982</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>7.4503105875500388</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F14" s="3">
         <f t="shared" si="1"/>
         <v>2.4444880200636652</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>19.190000000000001</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>75</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <f t="shared" si="3"/>
         <v>2.2576079434169878</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>22.124557845486482</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F15" s="3">
         <f t="shared" si="1"/>
         <v>7.2591895286719872</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B16" s="5">
         <v>65</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <f t="shared" si="3"/>
         <v>3.6863838376381919</v>
       </c>
-      <c r="D15" s="2">
-        <f t="shared" ref="D15:D24" si="4">C15*9.8</f>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:D26" si="4">C16*9.8</f>
         <v>36.126561608854281</v>
       </c>
-      <c r="F15" s="3">
-        <f t="shared" ref="F15:F24" si="5">D15/$E$2</f>
+      <c r="F16" s="3">
+        <f t="shared" ref="F16:F26" si="5">D16/$E$2</f>
         <v>11.853324236778752</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
         <v>3.49</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B17" s="5">
         <v>55</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <f t="shared" si="3"/>
         <v>5.0031508243529892</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <f t="shared" si="4"/>
         <v>49.030878078659299</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F17" s="3">
         <f t="shared" si="5"/>
         <v>16.087301686022474</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B18" s="17">
         <v>45</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C18" s="18">
         <f t="shared" si="3"/>
         <v>6.1678996049862942</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D18" s="18">
         <f t="shared" si="4"/>
         <v>60.445416128865688</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20">
+      <c r="E18" s="19"/>
+      <c r="F18" s="20">
         <f t="shared" si="5"/>
         <v>19.832474614103841</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
-        <f>A16*4</f>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <f>A17*4</f>
         <v>13.96</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B19" s="5">
         <v>35</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <f t="shared" si="3"/>
         <v>7.1452398772298871</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <f t="shared" si="4"/>
         <v>70.023350796852895</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F19" s="3">
         <f t="shared" si="5"/>
         <v>22.975047836752047</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="5">
+        <v>27.5</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="3"/>
+        <v>7.7371535857682154</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="4"/>
+        <v>75.824105140528516</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="5"/>
+        <v>24.878307349737028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
         <v>25</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C21" s="2">
         <f t="shared" si="3"/>
         <v>7.9054756514696871</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <f t="shared" si="4"/>
         <v>77.473661384402945</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F21" s="3">
         <f t="shared" si="5"/>
         <v>25.419535856815717</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
         <v>15</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C22" s="2">
         <f t="shared" si="3"/>
         <v>8.4255075484032815</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D22" s="2">
         <f t="shared" si="4"/>
         <v>82.569973974352166</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F22" s="3">
         <f t="shared" si="5"/>
         <v>27.091664142775826</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="9">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9">
         <v>0</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C23" s="10">
         <f t="shared" si="3"/>
         <v>8.7227272727272727</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D23" s="10">
         <f t="shared" si="4"/>
         <v>85.482727272727274</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="11">
+      <c r="E23" s="8"/>
+      <c r="F23" s="11">
         <f t="shared" si="5"/>
         <v>28.047354574685766</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B24" s="1">
         <v>90</v>
       </c>
-      <c r="C22" s="2">
-        <f>($A$24/2.2)*COS(RADIANS(B22))</f>
+      <c r="C24" s="2">
+        <f>($A$26/2.2)*COS(RADIANS(B24))</f>
         <v>7.7407106923771895E-16</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D24" s="2">
         <f t="shared" si="4"/>
         <v>7.5858964785296464E-15</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E24" s="2">
         <f>0.311*9.8</f>
         <v>3.0478000000000001</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F24" s="3">
         <f t="shared" si="5"/>
         <v>2.4889744991566527E-15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1">
-        <v>85</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" ref="C23:C31" si="6">($A$24/2.2)*COS(RADIANS(B23))</f>
-        <v>1.1013316583567709</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="4"/>
-        <v>10.793050251896355</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="5"/>
-        <v>3.5412593516294883</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>27.8</v>
-      </c>
-      <c r="B24" s="1">
-        <v>75</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" si="6"/>
-        <v>3.2705315699318525</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="4"/>
-        <v>32.051209385332157</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="5"/>
-        <v>10.516178681452903</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1">
+        <v>85</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:C33" si="6">($A$26/2.2)*COS(RADIANS(B25))</f>
+        <v>1.1013316583567709</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="4"/>
+        <v>10.793050251896355</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="5"/>
+        <v>3.5412593516294883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>75</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="6"/>
+        <v>3.2705315699318525</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="4"/>
+        <v>32.051209385332157</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="5"/>
+        <v>10.516178681452903</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B27" s="5">
         <v>65</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C27" s="2">
         <f t="shared" si="6"/>
         <v>5.3403580347233834</v>
       </c>
-      <c r="D25" s="2">
-        <f t="shared" ref="D25:D41" si="7">C25*9.8</f>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D43" si="7">C27*9.8</f>
         <v>52.335508740289164</v>
       </c>
-      <c r="F25" s="3">
-        <f t="shared" ref="F25:F41" si="8">D25/$E$2</f>
+      <c r="F27" s="3">
+        <f t="shared" ref="F27:F43" si="8">D27/$E$2</f>
         <v>17.17156924348355</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
         <v>5.92</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B28" s="5">
         <v>55</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C28" s="2">
         <f t="shared" si="6"/>
         <v>7.2479204229814007</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D28" s="2">
         <f t="shared" si="7"/>
         <v>71.029620145217734</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F28" s="3">
         <f t="shared" si="8"/>
         <v>23.30521036328425</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B29" s="17">
         <v>45</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C29" s="18">
         <f t="shared" si="6"/>
         <v>8.935258416811827</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D29" s="18">
         <f t="shared" si="7"/>
         <v>87.565532484755906</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="20">
+      <c r="E29" s="19"/>
+      <c r="F29" s="20">
         <f t="shared" si="8"/>
         <v>28.730734459202015</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="16">
-        <f>A26*4</f>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <f>A28*4</f>
         <v>23.68</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B30" s="5">
         <v>35</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C30" s="2">
         <f t="shared" si="6"/>
         <v>10.35110310510635</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D30" s="2">
         <f t="shared" si="7"/>
         <v>101.44081043004225</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F30" s="3">
         <f t="shared" si="8"/>
         <v>33.283289727030066</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
         <v>25</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C31" s="2">
         <f t="shared" si="6"/>
         <v>11.452434763463121</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D31" s="2">
         <f t="shared" si="7"/>
         <v>112.23386068193859</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F31" s="3">
         <f t="shared" si="8"/>
         <v>36.824549078659558</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
         <v>15</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C32" s="2">
         <f t="shared" si="6"/>
         <v>12.20578998674368</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D32" s="2">
         <f t="shared" si="7"/>
         <v>119.61674187008808</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F32" s="3">
         <f t="shared" si="8"/>
         <v>39.246913140654925</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="9">
+    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="9">
         <v>0</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C33" s="10">
         <f t="shared" si="6"/>
         <v>12.636363636363635</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D33" s="10">
         <f t="shared" si="7"/>
         <v>123.83636363636363</v>
       </c>
-      <c r="E31" s="8"/>
-      <c r="F31" s="11">
+      <c r="E33" s="8"/>
+      <c r="F33" s="11">
         <f t="shared" si="8"/>
         <v>40.631394329143525</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B34" s="1">
         <v>90</v>
       </c>
-      <c r="C32" s="2">
-        <f>($A$34/2.2)*COS(RADIANS(B32))</f>
+      <c r="C34" s="2">
+        <f>($A$36/2.2)*COS(RADIANS(B34))</f>
         <v>3.1519728430830858E-16</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D34" s="2">
         <f t="shared" si="7"/>
         <v>3.0889333862214242E-15</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E34" s="2">
         <f>0.311*9.8</f>
         <v>3.0478000000000001</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F34" s="3">
         <f t="shared" si="8"/>
         <v>1.0134960910235002E-15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="1">
-        <v>85</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" ref="C33:C41" si="9">($A$34/2.2)*COS(RADIANS(B33))</f>
-        <v>0.44845591268340462</v>
-      </c>
-      <c r="D33" s="2">
-        <f t="shared" si="7"/>
-        <v>4.3948679442973653</v>
-      </c>
-      <c r="F33" s="3">
-        <f t="shared" si="8"/>
-        <v>1.4419804266347416</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
-        <v>11.32</v>
-      </c>
-      <c r="B34" s="1">
-        <v>75</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" si="9"/>
-        <v>1.3317416320729705</v>
-      </c>
-      <c r="D34" s="2">
-        <f t="shared" si="7"/>
-        <v>13.051067994315112</v>
-      </c>
-      <c r="F34" s="3">
-        <f t="shared" si="8"/>
-        <v>4.282127434318233</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1">
+        <v>85</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" ref="C35:C43" si="9">($A$36/2.2)*COS(RADIANS(B35))</f>
+        <v>0.44845591268340462</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="7"/>
+        <v>4.3948679442973653</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="8"/>
+        <v>1.4419804266347416</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>11.32</v>
+      </c>
+      <c r="B36" s="1">
+        <v>75</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="9"/>
+        <v>1.3317416320729705</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="7"/>
+        <v>13.051067994315112</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="8"/>
+        <v>4.282127434318233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B37" s="5">
         <v>65</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C37" s="2">
         <f t="shared" si="9"/>
         <v>2.1745630558657809</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D37" s="2">
         <f t="shared" si="7"/>
         <v>21.310717947484655</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F37" s="3">
         <f t="shared" si="8"/>
         <v>6.9921641667710004</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
         <v>1.71</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B38" s="5">
         <v>55</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C38" s="2">
         <f t="shared" si="9"/>
         <v>2.9513114815881103</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D38" s="2">
         <f t="shared" si="7"/>
         <v>28.922852519563484</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F38" s="3">
         <f t="shared" si="8"/>
         <v>9.4897475292222211</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B39" s="17">
         <v>45</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C39" s="18">
         <f t="shared" si="9"/>
         <v>3.6383858013780541</v>
       </c>
-      <c r="D37" s="18">
+      <c r="D39" s="18">
         <f t="shared" si="7"/>
         <v>35.656180853504935</v>
       </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20">
+      <c r="E39" s="19"/>
+      <c r="F39" s="20">
         <f t="shared" si="8"/>
         <v>11.698989715041977</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="16">
-        <f>A36*4</f>
+    <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
+        <f>A38*4</f>
         <v>6.84</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B40" s="5">
         <v>35</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C40" s="2">
         <f t="shared" si="9"/>
         <v>4.2149096097051757</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D40" s="2">
         <f t="shared" si="7"/>
         <v>41.306114175110721</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F40" s="3">
         <f t="shared" si="8"/>
         <v>13.552764018344616</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="1">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
         <v>25</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C41" s="2">
         <f t="shared" si="9"/>
         <v>4.663365522388581</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D41" s="2">
         <f t="shared" si="7"/>
         <v>45.700982119408096</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F41" s="3">
         <f t="shared" si="8"/>
         <v>14.994744444979361</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="1">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
         <v>15</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C42" s="2">
         <f t="shared" si="9"/>
         <v>4.9701274334510241</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D42" s="2">
         <f t="shared" si="7"/>
         <v>48.70724884782004</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F42" s="3">
         <f t="shared" si="8"/>
         <v>15.981117149360207</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="9">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9">
         <v>0</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C43" s="10">
         <f t="shared" si="9"/>
         <v>5.1454545454545455</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D43" s="10">
         <f t="shared" si="7"/>
         <v>50.425454545454549</v>
       </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="11">
+      <c r="E43" s="8"/>
+      <c r="F43" s="11">
         <f t="shared" si="8"/>
         <v>16.544869921075708</v>
       </c>

</xml_diff>

<commit_message>
add new prototype, edit misc excel
</commit_message>
<xml_diff>
--- a/force_calculations.xlsx
+++ b/force_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdaha\Documents\GitHub\commapogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474A5CD8-9C75-48C8-AB9F-D99D0352E514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BF7466-10FE-40CD-9481-50ED96C9B6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{6BFD6DE9-8C03-4167-ADB1-1BE53FC596A2}"/>
   </bookViews>
@@ -3261,7 +3261,7 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="6635462" y="1565563"/>
+    <xdr:pos x="6083012" y="1689388"/>
     <xdr:ext cx="6166138" cy="4216112"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3624,7 +3624,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F9"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>